<commit_message>
Updated country domain for US
</commit_message>
<xml_diff>
--- a/Documentation Service/Documentation model/resources/domains/dynamicDomainTemplate.xlsx
+++ b/Documentation Service/Documentation model/resources/domains/dynamicDomainTemplate.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hhdiazlo/Desktop/2BDeleted/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cp4a/ITZ-CP4BA-cluster/deployments/cp4ba-v2/backups/backup_29Apr2024/ADS/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{383AE2B9-69ED-5947-8856-4D588B85FF42}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C539251D-B5A8-454F-9E55-8295ED5AA41E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="29040" windowHeight="16940" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KYCDocumentsDomain" sheetId="1" r:id="rId1"/>
@@ -169,9 +169,6 @@
     <t>UK</t>
   </si>
   <si>
-    <t>USA</t>
-  </si>
-  <si>
     <t>BROKERDEALER</t>
   </si>
   <si>
@@ -251,6 +248,9 @@
   </si>
   <si>
     <t>WolfsbergQuestionnaire</t>
+  </si>
+  <si>
+    <t>US</t>
   </si>
 </sst>
 </file>
@@ -314,9 +314,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -354,7 +354,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -460,7 +460,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -602,7 +602,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -612,7 +612,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
+    <sheetView zoomScale="153" zoomScaleNormal="153" workbookViewId="0">
       <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
@@ -636,7 +636,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -644,7 +644,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B3" t="s">
         <v>4</v>
@@ -652,7 +652,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B4" t="s">
         <v>5</v>
@@ -660,7 +660,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B5" t="s">
         <v>6</v>
@@ -676,7 +676,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>8</v>
@@ -684,7 +684,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>9</v>
@@ -692,7 +692,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B9" t="s">
         <v>10</v>
@@ -700,7 +700,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B10" t="s">
         <v>11</v>
@@ -708,7 +708,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B11" t="s">
         <v>12</v>
@@ -716,7 +716,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B12" t="s">
         <v>13</v>
@@ -724,15 +724,15 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" t="s">
         <v>61</v>
-      </c>
-      <c r="B13" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B14" t="s">
         <v>14</v>
@@ -740,7 +740,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B15" t="s">
         <v>15</v>
@@ -748,7 +748,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B16" t="s">
         <v>16</v>
@@ -756,7 +756,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B17" t="s">
         <v>17</v>
@@ -764,7 +764,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B18" t="s">
         <v>18</v>
@@ -772,7 +772,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B19" t="s">
         <v>19</v>
@@ -780,7 +780,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B20" t="s">
         <v>20</v>
@@ -788,7 +788,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B21" t="s">
         <v>21</v>
@@ -796,7 +796,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B22" t="s">
         <v>22</v>
@@ -835,7 +835,7 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B2" t="s">
         <v>29</v>
@@ -843,7 +843,7 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B3" t="s">
         <v>30</v>
@@ -851,7 +851,7 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B4" t="s">
         <v>31</v>
@@ -867,7 +867,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B6" t="s">
         <v>33</v>
@@ -883,7 +883,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B8" t="s">
         <v>35</v>
@@ -899,7 +899,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B10" t="s">
         <v>37</v>
@@ -922,8 +922,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D710C59-05DC-E94D-AFB1-81D207E04006}">
   <dimension ref="A1:C7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -984,7 +984,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
       <c r="B7" t="s">
         <v>28</v>

</xml_diff>